<commit_message>
Updated Sprint Backlog after scrum on day 2
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint 2 Backlog.xlsx
+++ b/Sprint 2/Sprint 2 Backlog.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Documents\Year 3\Semester 2\Agile\AgileGroup4\Sprint 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smith\Documents\AgileGroup4\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B67A4E-FD25-4C09-BF00-A21632EB5AF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
   <si>
     <t>Product Backlog Story</t>
   </si>
@@ -145,12 +156,15 @@
   </si>
   <si>
     <t>Aditya, Tom</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -629,24 +643,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="54.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
     <col min="10" max="10" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>13</v>
       </c>
@@ -696,7 +710,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -707,7 +721,7 @@
         <v>40</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="5"/>
@@ -717,7 +731,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>18</v>
       </c>
@@ -738,7 +752,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -759,7 +773,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -772,7 +786,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>21</v>
       </c>
@@ -790,7 +804,7 @@
       <c r="J7" s="13"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>16</v>
       </c>
@@ -811,7 +825,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>20</v>
       </c>
@@ -832,7 +846,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="8"/>
       <c r="C10" s="6"/>
@@ -845,7 +859,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>22</v>
       </c>
@@ -862,7 +876,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>23</v>
       </c>
@@ -873,7 +887,7 @@
         <v>39</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -883,7 +897,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>24</v>
       </c>
@@ -904,7 +918,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>25</v>
       </c>
@@ -925,7 +939,7 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="8"/>
       <c r="C15" s="5"/>
@@ -938,7 +952,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>26</v>
       </c>
@@ -956,7 +970,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>28</v>
       </c>
@@ -967,7 +981,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -977,7 +991,7 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>27</v>
       </c>
@@ -998,7 +1012,7 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
         <v>29</v>
       </c>
@@ -1019,7 +1033,7 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>30</v>
       </c>
@@ -1035,7 +1049,7 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>31</v>
       </c>
@@ -1046,7 +1060,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -1055,7 +1069,7 @@
       <c r="I22" s="6"/>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>33</v>
       </c>
@@ -1075,7 +1089,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
         <v>32</v>
       </c>
@@ -1095,7 +1109,7 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>34</v>
       </c>
@@ -1112,7 +1126,7 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
         <v>35</v>
       </c>
@@ -1123,7 +1137,7 @@
         <v>38</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
@@ -1132,7 +1146,7 @@
       <c r="I27" s="6"/>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
         <v>36</v>
       </c>
@@ -1152,7 +1166,7 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>37</v>
       </c>
@@ -1234,7 +1248,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D3:D6 D17:D19 D12:D14 D8:D9 D22:D24 D27:D29">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D3:D6 D17:D19 D12:D14 D8:D9 D22:D24 D27:D29" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Done,In progress,Not started"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added Sprint story points
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint 2 Backlog.xlsx
+++ b/Sprint 2/Sprint 2 Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Github\AgileGroup4\Sprint 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EXTERMINATOR\Desktop\Projects\AgileGroup4\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5612F2C-D8E9-4828-A3CE-B4C439D801AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5635E0CB-2D64-4026-893B-C38B4C0C489D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -732,8 +732,8 @@
   </sheetPr>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -860,8 +860,15 @@
       <c r="F5">
         <v>3</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2</v>
+      </c>
+      <c r="I5" s="5">
+        <v>2</v>
+      </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
     </row>
@@ -1424,15 +1431,15 @@
       </c>
       <c r="G34" s="32">
         <f>SUM(G3:G32)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H34" s="32">
-        <f t="shared" ref="G34:I34" si="0">SUM(H3:H32)</f>
-        <v>11</v>
+        <f t="shared" ref="H34" si="0">SUM(H3:H32)</f>
+        <v>13</v>
       </c>
       <c r="I34" s="32">
         <f>SUM(I3:I33)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>